<commit_message>
Published state of ETDataset on 1 August 2014.
</commit_message>
<xml_diff>
--- a/analyses/6_residences_analysis.xlsx
+++ b/analyses/6_residences_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15300" tabRatio="932" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="932" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="876">
   <si>
     <t>Changelog</t>
   </si>
@@ -2268,12 +2268,6 @@
   </si>
   <si>
     <t>Added parent_share that fixes problem in the graph https://github.com/quintel/refinery/issues/37</t>
-  </si>
-  <si>
-    <t>Useful heat in space heating coming from electric heater add on (if a household is equipped)</t>
-  </si>
-  <si>
-    <t>Useful heat in hot water preparation coming from electric heater add on (if a household is equipped)</t>
   </si>
   <si>
     <t>results form ETM modelling logic</t>
@@ -2725,12 +2719,6 @@
     <t>Percentage of useful heat in space heating delivered by</t>
   </si>
   <si>
-    <t>Useful heat in space heating delivered from solar thermal panel (if a household is equipped)</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>improved text of intro sheet</t>
   </si>
   <si>
@@ -2738,12 +2726,6 @@
   </si>
   <si>
     <t>value</t>
-  </si>
-  <si>
-    <t>Percent of old houses (built before 1992)</t>
-  </si>
-  <si>
-    <t>Percent of new houses (built after 1991)</t>
   </si>
   <si>
     <t xml:space="preserve">The main goal of this analysis is to provide a breakdown of the residential energy consumption. Energy is consumed in the applications space heating, hot water, space cooling, lighting, cooking and electric applications. Furthermore, the energy use within these applications is split over certain technologies (for example: coal, gas and oil heaters in space heating). 
@@ -2772,6 +2754,24 @@
   </si>
   <si>
     <t>Correct misstake in application share calculation for district heat</t>
+  </si>
+  <si>
+    <t>Percentage of old houses (built before 1992)</t>
+  </si>
+  <si>
+    <t>Percentage of new houses (built after 1991)</t>
+  </si>
+  <si>
+    <t>electricity-driven heat pump (air)</t>
+  </si>
+  <si>
+    <t>Percentage of useful heat in space heating delivered by solar thermal panel (if household is equipped)</t>
+  </si>
+  <si>
+    <t>Percentage of useful heat in hot water delivered by electric heater add on (if household is equipped)</t>
+  </si>
+  <si>
+    <t>Percentage of useful heat in space heating delivered by electric heater add on (if household is equipped)</t>
   </si>
 </sst>
 </file>
@@ -13475,7 +13475,7 @@
     <row r="30" spans="2:4" ht="60">
       <c r="B30" s="20"/>
       <c r="C30" s="470" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D30" s="7"/>
     </row>
@@ -13902,7 +13902,7 @@
     <row r="32" spans="2:6">
       <c r="B32" s="176"/>
       <c r="C32" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D32" s="346">
         <f>SUM('Final demand per energy carrier'!F65:F72)</f>
@@ -13937,7 +13937,7 @@
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="482" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C35" s="342"/>
       <c r="D35" s="348"/>
@@ -14824,7 +14824,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="B5" s="647" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C5" s="657"/>
       <c r="D5" s="20"/>
@@ -14845,7 +14845,7 @@
     <row r="7" spans="1:10">
       <c r="A7" s="164"/>
       <c r="B7" s="165" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C7" s="166"/>
       <c r="D7" s="167"/>
@@ -14885,10 +14885,10 @@
       <c r="B10" s="172"/>
       <c r="C10" s="173"/>
       <c r="D10" s="173" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E10" s="557" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F10" s="158"/>
       <c r="G10" s="158"/>
@@ -14899,7 +14899,7 @@
     <row r="11" spans="1:10">
       <c r="A11" s="164"/>
       <c r="B11" s="562" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C11" s="106"/>
       <c r="D11" s="274">
@@ -14923,7 +14923,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="31" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="559">
@@ -14947,7 +14947,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="31" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="559" t="e">
@@ -14970,7 +14970,7 @@
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="31" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="559" t="e">
@@ -14994,7 +14994,7 @@
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="31" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="298" t="e">
@@ -15254,13 +15254,13 @@
         <v>399</v>
       </c>
       <c r="E9" s="65" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F9" s="65" t="s">
         <v>436</v>
       </c>
       <c r="G9" s="65" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="H9" s="65" t="s">
         <v>437</v>
@@ -15272,7 +15272,7 @@
         <v>439</v>
       </c>
       <c r="K9" s="113" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -16563,7 +16563,7 @@
     <row r="76" spans="2:13">
       <c r="B76" s="36"/>
       <c r="C76" s="508" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D76" s="509"/>
       <c r="E76" s="507" t="e">
@@ -16599,7 +16599,7 @@
     <row r="77" spans="2:13">
       <c r="B77" s="36"/>
       <c r="C77" s="511" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D77" s="510"/>
       <c r="E77" s="507" t="e">
@@ -16635,7 +16635,7 @@
     <row r="78" spans="2:13">
       <c r="B78" s="36"/>
       <c r="C78" s="512" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D78" s="513"/>
       <c r="E78" s="514" t="e">
@@ -18540,7 +18540,7 @@
       <c r="B24" s="467"/>
       <c r="C24" s="467"/>
       <c r="K24" s="658" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="L24" s="659"/>
     </row>
@@ -18615,7 +18615,7 @@
   <sheetData>
     <row r="2" spans="1:13" ht="20">
       <c r="B2" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -20403,7 +20403,7 @@
         <v>41500</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D20" s="27">
         <v>2.04</v>
@@ -20414,7 +20414,7 @@
         <v>41505</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D21" s="27">
         <v>2.0499999999999998</v>
@@ -20425,7 +20425,7 @@
         <v>41507</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>483</v>
@@ -20436,7 +20436,7 @@
         <v>41507</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D23" s="27">
         <v>2.06</v>
@@ -20447,7 +20447,7 @@
         <v>41512</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D24" s="27">
         <v>2.0699999999999998</v>
@@ -20458,7 +20458,7 @@
         <v>41534</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D25" s="27">
         <v>2.08</v>
@@ -20469,7 +20469,7 @@
         <v>41535</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D26" s="27">
         <v>2.09</v>
@@ -20480,7 +20480,7 @@
         <v>41535</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D27" s="27">
         <v>2.1</v>
@@ -20491,7 +20491,7 @@
         <v>41561</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D28" s="18">
         <v>2.11</v>
@@ -20502,7 +20502,7 @@
         <v>41562</v>
       </c>
       <c r="C29" s="625" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D29" s="18">
         <v>2.12</v>
@@ -20513,7 +20513,7 @@
         <v>41578</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D30" s="18">
         <v>2.13</v>
@@ -20524,7 +20524,7 @@
         <v>41618</v>
       </c>
       <c r="C31" s="40" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="D31" s="18">
         <v>2.14</v>
@@ -20532,10 +20532,10 @@
     </row>
     <row r="32" spans="2:4" ht="30">
       <c r="B32" s="408" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="D32" s="18">
         <v>2.15</v>
@@ -20543,10 +20543,10 @@
     </row>
     <row r="33" spans="2:4" ht="30">
       <c r="B33" s="408" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="D33" s="18">
         <v>2.16</v>
@@ -20554,10 +20554,10 @@
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="408" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="D34" s="18">
         <v>2.17</v>
@@ -21130,7 +21130,7 @@
         <v>493</v>
       </c>
       <c r="B1" s="466" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -21409,7 +21409,7 @@
     </row>
     <row r="13" spans="2:3" ht="28" customHeight="1">
       <c r="B13" s="490" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C13" s="488" t="s">
         <v>225</v>
@@ -21465,7 +21465,7 @@
     </row>
     <row r="20" spans="2:3" ht="28" customHeight="1">
       <c r="B20" s="493" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C20" s="488" t="s">
         <v>223</v>
@@ -21489,7 +21489,7 @@
     </row>
     <row r="23" spans="2:3" ht="28" customHeight="1">
       <c r="B23" s="494" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C23" s="488" t="s">
         <v>224</v>
@@ -21732,7 +21732,7 @@
         <v>709</v>
       </c>
       <c r="C53" s="498" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D53" s="20"/>
     </row>
@@ -22463,7 +22463,7 @@
     </row>
     <row r="6" spans="2:2" ht="90">
       <c r="B6" s="87" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
     </row>
     <row r="7" spans="2:2">
@@ -22520,7 +22520,7 @@
     </row>
     <row r="20" spans="2:2" ht="90">
       <c r="B20" s="86" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
   </sheetData>
@@ -22910,7 +22910,7 @@
         <v>701</v>
       </c>
       <c r="B1" s="466" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -22967,7 +22967,7 @@
         <v>708</v>
       </c>
       <c r="B1" s="466" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -23022,7 +23022,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -23030,7 +23030,7 @@
         <v>532</v>
       </c>
       <c r="B2" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -23591,7 +23591,7 @@
     <row r="16" spans="2:4" ht="15" customHeight="1">
       <c r="B16" s="39"/>
       <c r="C16" s="74" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D16" s="41"/>
     </row>
@@ -23606,7 +23606,7 @@
         <v>482</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="14" customHeight="1">
@@ -23627,7 +23627,7 @@
         <v>510</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="14" customHeight="1">
@@ -23636,7 +23636,7 @@
         <v>511</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="14" customHeight="1">
@@ -23645,7 +23645,7 @@
         <v>512</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="14" customHeight="1">
@@ -23654,7 +23654,7 @@
         <v>513</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="14" customHeight="1">
@@ -23665,7 +23665,7 @@
     <row r="26" spans="2:4" ht="75">
       <c r="B26" s="39"/>
       <c r="C26" s="40" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D26" s="41"/>
     </row>
@@ -23677,10 +23677,10 @@
     <row r="28" spans="2:4" ht="14" customHeight="1">
       <c r="B28" s="39"/>
       <c r="C28" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="14" customHeight="1">
@@ -23691,10 +23691,10 @@
     <row r="30" spans="2:4" ht="14" customHeight="1">
       <c r="B30" s="39"/>
       <c r="C30" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="14" customHeight="1">
@@ -23707,21 +23707,21 @@
     <row r="32" spans="2:4" ht="14" customHeight="1">
       <c r="B32" s="39"/>
       <c r="C32" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D32" s="41"/>
     </row>
     <row r="33" spans="2:4" ht="14" customHeight="1">
       <c r="B33" s="39"/>
       <c r="C33" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D33" s="41"/>
     </row>
     <row r="34" spans="2:4" ht="14" customHeight="1">
       <c r="B34" s="39"/>
       <c r="C34" s="17" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D34" s="41"/>
     </row>
@@ -24851,7 +24851,7 @@
     </row>
     <row r="182" spans="2:3">
       <c r="B182" s="49" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C182" s="43" t="s">
         <v>104</v>
@@ -24918,7 +24918,7 @@
         <v>27</v>
       </c>
       <c r="I2" s="454" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="4"/>
@@ -25011,7 +25011,7 @@
       </c>
       <c r="F9" s="564"/>
       <c r="G9" s="564" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="H9" s="564"/>
       <c r="I9" s="564" t="s">
@@ -25029,7 +25029,7 @@
       </c>
       <c r="N9" s="15"/>
       <c r="O9" s="464" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="P9" s="465" t="s">
         <v>690</v>
@@ -25068,7 +25068,7 @@
       <c r="E11" s="71"/>
       <c r="F11" s="194"/>
       <c r="G11" s="23" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -25203,7 +25203,7 @@
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="652" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="L17" s="356"/>
       <c r="M17" s="357"/>
@@ -25231,7 +25231,7 @@
     <row r="19" spans="2:16" ht="16" customHeight="1" thickBot="1">
       <c r="B19" s="38"/>
       <c r="C19" s="630" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D19" s="398"/>
       <c r="E19" s="270"/>
@@ -25468,7 +25468,7 @@
     <row r="27" spans="2:16">
       <c r="B27" s="38"/>
       <c r="C27" s="194" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D27" s="398" t="s">
         <v>214</v>
@@ -25547,7 +25547,7 @@
     <row r="30" spans="2:16" ht="16" customHeight="1" thickBot="1">
       <c r="B30" s="38"/>
       <c r="C30" s="630" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D30" s="398"/>
       <c r="E30" s="257"/>
@@ -25566,7 +25566,7 @@
     <row r="31" spans="2:16" ht="16" thickBot="1">
       <c r="B31" s="38"/>
       <c r="C31" s="629" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D31" s="401"/>
       <c r="E31" s="395"/>
@@ -25587,7 +25587,7 @@
     <row r="32" spans="2:16" ht="16" thickBot="1">
       <c r="B32" s="38"/>
       <c r="C32" s="629" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D32" s="401"/>
       <c r="E32" s="395"/>
@@ -25608,7 +25608,7 @@
     <row r="33" spans="2:16" ht="16" thickBot="1">
       <c r="B33" s="38"/>
       <c r="C33" s="629" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D33" s="401"/>
       <c r="E33" s="395"/>
@@ -25629,7 +25629,7 @@
     <row r="34" spans="2:16" ht="16" thickBot="1">
       <c r="B34" s="38"/>
       <c r="C34" s="629" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D34" s="401"/>
       <c r="E34" s="395"/>
@@ -25650,7 +25650,7 @@
     <row r="35" spans="2:16" ht="16" thickBot="1">
       <c r="B35" s="38"/>
       <c r="C35" s="629" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D35" s="401"/>
       <c r="E35" s="395"/>
@@ -25671,7 +25671,7 @@
     <row r="36" spans="2:16" ht="16" thickBot="1">
       <c r="B36" s="38"/>
       <c r="C36" s="629" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D36" s="401"/>
       <c r="E36" s="395"/>
@@ -25692,7 +25692,7 @@
     <row r="37" spans="2:16" ht="16" thickBot="1">
       <c r="B37" s="38"/>
       <c r="C37" s="629" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D37" s="401"/>
       <c r="E37" s="395"/>
@@ -25713,7 +25713,7 @@
     <row r="38" spans="2:16" ht="16" thickBot="1">
       <c r="B38" s="38"/>
       <c r="C38" s="629" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D38" s="401"/>
       <c r="E38" s="395"/>
@@ -25734,7 +25734,7 @@
     <row r="39" spans="2:16" ht="16" thickBot="1">
       <c r="B39" s="38"/>
       <c r="C39" s="629" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D39" s="401"/>
       <c r="E39" s="395"/>
@@ -25757,7 +25757,7 @@
     <row r="40" spans="2:16" ht="16" thickBot="1">
       <c r="B40" s="38"/>
       <c r="C40" s="629" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D40" s="401"/>
       <c r="E40" s="395"/>
@@ -25774,7 +25774,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M40" s="357" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="N40" s="75"/>
       <c r="O40" s="461" t="s">
@@ -25785,7 +25785,7 @@
     <row r="41" spans="2:16" ht="16" thickBot="1">
       <c r="B41" s="38"/>
       <c r="C41" s="629" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D41" s="401"/>
       <c r="E41" s="395"/>
@@ -25878,7 +25878,7 @@
     <row r="45" spans="2:16" ht="16" customHeight="1" thickBot="1">
       <c r="B45" s="38"/>
       <c r="C45" s="630" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D45" s="398"/>
       <c r="E45" s="261"/>
@@ -25897,7 +25897,7 @@
     <row r="46" spans="2:16" ht="16" thickBot="1">
       <c r="B46" s="38"/>
       <c r="C46" s="629" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D46" s="401"/>
       <c r="E46" s="395"/>
@@ -25918,7 +25918,7 @@
     <row r="47" spans="2:16" ht="16" thickBot="1">
       <c r="B47" s="38"/>
       <c r="C47" s="629" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D47" s="401"/>
       <c r="E47" s="395"/>
@@ -25939,7 +25939,7 @@
     <row r="48" spans="2:16" ht="16" thickBot="1">
       <c r="B48" s="38"/>
       <c r="C48" s="629" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="D48" s="401"/>
       <c r="E48" s="395"/>
@@ -25960,7 +25960,7 @@
     <row r="49" spans="2:16" ht="16" thickBot="1">
       <c r="B49" s="38"/>
       <c r="C49" s="629" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D49" s="401"/>
       <c r="E49" s="395"/>
@@ -25981,7 +25981,7 @@
     <row r="50" spans="2:16" ht="16" thickBot="1">
       <c r="B50" s="38"/>
       <c r="C50" s="629" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D50" s="401"/>
       <c r="E50" s="395"/>
@@ -26002,7 +26002,7 @@
     <row r="51" spans="2:16" ht="16" thickBot="1">
       <c r="B51" s="38"/>
       <c r="C51" s="629" t="s">
-        <v>387</v>
+        <v>872</v>
       </c>
       <c r="D51" s="401"/>
       <c r="E51" s="395"/>
@@ -26023,7 +26023,7 @@
     <row r="52" spans="2:16" ht="16" thickBot="1">
       <c r="B52" s="38"/>
       <c r="C52" s="629" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D52" s="401"/>
       <c r="E52" s="395"/>
@@ -26044,7 +26044,7 @@
     <row r="53" spans="2:16" ht="16" thickBot="1">
       <c r="B53" s="38"/>
       <c r="C53" s="629" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="D53" s="401"/>
       <c r="E53" s="395"/>
@@ -26065,7 +26065,7 @@
     <row r="54" spans="2:16" ht="16" thickBot="1">
       <c r="B54" s="38"/>
       <c r="C54" s="629" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D54" s="401"/>
       <c r="E54" s="395"/>
@@ -26086,7 +26086,7 @@
     <row r="55" spans="2:16" ht="16" thickBot="1">
       <c r="B55" s="38"/>
       <c r="C55" s="629" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D55" s="401"/>
       <c r="E55" s="395"/>
@@ -26107,7 +26107,7 @@
     <row r="56" spans="2:16" ht="16" thickBot="1">
       <c r="B56" s="38"/>
       <c r="C56" s="629" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D56" s="401"/>
       <c r="E56" s="395"/>
@@ -26128,7 +26128,7 @@
     <row r="57" spans="2:16" ht="16" thickBot="1">
       <c r="B57" s="38"/>
       <c r="C57" s="629" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D57" s="401"/>
       <c r="E57" s="395"/>
@@ -26196,7 +26196,7 @@
     <row r="60" spans="2:16" ht="16" thickBot="1">
       <c r="B60" s="38"/>
       <c r="C60" s="630" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D60" s="402"/>
       <c r="E60" s="639"/>
@@ -26215,7 +26215,7 @@
     <row r="61" spans="2:16" ht="16" thickBot="1">
       <c r="B61" s="38"/>
       <c r="C61" s="629" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D61" s="403"/>
       <c r="E61" s="396"/>
@@ -26236,7 +26236,7 @@
     <row r="62" spans="2:16" ht="16" thickBot="1">
       <c r="B62" s="38"/>
       <c r="C62" s="629" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D62" s="403"/>
       <c r="E62" s="396"/>
@@ -26257,7 +26257,7 @@
     <row r="63" spans="2:16" ht="16" thickBot="1">
       <c r="B63" s="38"/>
       <c r="C63" s="629" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D63" s="404"/>
       <c r="E63" s="396"/>
@@ -26325,7 +26325,7 @@
     <row r="66" spans="2:16" ht="16" thickBot="1">
       <c r="B66" s="38"/>
       <c r="C66" s="630" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D66" s="398"/>
       <c r="E66" s="639"/>
@@ -26344,7 +26344,7 @@
     <row r="67" spans="2:16" ht="16" thickBot="1">
       <c r="B67" s="38"/>
       <c r="C67" s="629" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D67" s="403"/>
       <c r="E67" s="396"/>
@@ -26365,7 +26365,7 @@
     <row r="68" spans="2:16" ht="16" thickBot="1">
       <c r="B68" s="38"/>
       <c r="C68" s="629" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D68" s="403"/>
       <c r="E68" s="396"/>
@@ -26454,7 +26454,7 @@
     <row r="72" spans="2:16" ht="16" thickBot="1">
       <c r="B72" s="38"/>
       <c r="C72" s="630" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D72" s="398"/>
       <c r="E72" s="639"/>
@@ -26473,7 +26473,7 @@
     <row r="73" spans="2:16" ht="16" thickBot="1">
       <c r="B73" s="38"/>
       <c r="C73" s="629" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D73" s="403"/>
       <c r="E73" s="396"/>
@@ -26494,7 +26494,7 @@
     <row r="74" spans="2:16" ht="16" thickBot="1">
       <c r="B74" s="38"/>
       <c r="C74" s="629" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D74" s="403"/>
       <c r="E74" s="396"/>
@@ -26515,7 +26515,7 @@
     <row r="75" spans="2:16" ht="16" thickBot="1">
       <c r="B75" s="38"/>
       <c r="C75" s="629" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D75" s="403"/>
       <c r="E75" s="396"/>
@@ -26536,7 +26536,7 @@
     <row r="76" spans="2:16" ht="16" thickBot="1">
       <c r="B76" s="38"/>
       <c r="C76" s="629" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D76" s="403"/>
       <c r="E76" s="396"/>
@@ -26557,7 +26557,7 @@
     <row r="77" spans="2:16" ht="16" thickBot="1">
       <c r="B77" s="38"/>
       <c r="C77" s="629" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D77" s="403"/>
       <c r="E77" s="396"/>
@@ -26625,7 +26625,7 @@
     <row r="80" spans="2:16" ht="16" thickBot="1">
       <c r="B80" s="38"/>
       <c r="C80" s="630" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D80" s="398"/>
       <c r="E80" s="639"/>
@@ -26882,11 +26882,9 @@
     <row r="93" spans="2:16" ht="16" thickBot="1">
       <c r="B93" s="38"/>
       <c r="C93" s="71" t="s">
-        <v>860</v>
-      </c>
-      <c r="D93" s="403" t="s">
-        <v>861</v>
-      </c>
+        <v>873</v>
+      </c>
+      <c r="D93" s="403"/>
       <c r="E93" s="396"/>
       <c r="F93" s="413"/>
       <c r="G93" s="437"/>
@@ -26905,11 +26903,9 @@
     <row r="94" spans="2:16" ht="16" thickBot="1">
       <c r="B94" s="38"/>
       <c r="C94" s="71" t="s">
-        <v>717</v>
-      </c>
-      <c r="D94" s="403" t="s">
-        <v>861</v>
-      </c>
+        <v>874</v>
+      </c>
+      <c r="D94" s="403"/>
       <c r="E94" s="396"/>
       <c r="F94" s="413"/>
       <c r="G94" s="430"/>
@@ -26945,11 +26941,9 @@
     <row r="96" spans="2:16" ht="16" thickBot="1">
       <c r="B96" s="38"/>
       <c r="C96" s="71" t="s">
-        <v>716</v>
-      </c>
-      <c r="D96" s="403" t="s">
-        <v>861</v>
-      </c>
+        <v>875</v>
+      </c>
+      <c r="D96" s="403"/>
       <c r="E96" s="396"/>
       <c r="F96" s="413"/>
       <c r="G96" s="430"/>
@@ -27021,7 +27015,7 @@
     <row r="100" spans="2:16" ht="16" thickBot="1">
       <c r="B100" s="38"/>
       <c r="C100" s="71" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
       <c r="D100" s="403"/>
       <c r="E100" s="396"/>
@@ -27053,7 +27047,7 @@
     <row r="101" spans="2:16" ht="16" thickBot="1">
       <c r="B101" s="38"/>
       <c r="C101" s="71" t="s">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="D101" s="403"/>
       <c r="E101" s="396"/>
@@ -27090,10 +27084,10 @@
     <row r="103" spans="2:16" ht="17" thickBot="1">
       <c r="B103" s="73"/>
       <c r="C103" s="17" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D103" s="403" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E103" s="646"/>
       <c r="F103" s="413"/>
@@ -27105,17 +27099,17 @@
       <c r="L103" s="56"/>
       <c r="M103" s="32"/>
       <c r="O103" s="461" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="P103" s="7"/>
     </row>
     <row r="104" spans="2:16" ht="17" thickBot="1">
       <c r="B104" s="73"/>
       <c r="C104" s="17" t="s">
+        <v>751</v>
+      </c>
+      <c r="D104" s="403" t="s">
         <v>753</v>
-      </c>
-      <c r="D104" s="403" t="s">
-        <v>755</v>
       </c>
       <c r="E104" s="646"/>
       <c r="F104" s="413"/>
@@ -27127,7 +27121,7 @@
       <c r="L104" s="56"/>
       <c r="M104" s="32"/>
       <c r="O104" s="461" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="P104" s="7"/>
     </row>
@@ -27409,7 +27403,7 @@
   <sheetData>
     <row r="2" spans="2:67" ht="20">
       <c r="B2" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="3" spans="2:67" ht="15" customHeight="1">
@@ -34290,7 +34284,7 @@
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="595" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C5" s="596"/>
       <c r="D5" s="596"/>
@@ -34321,10 +34315,10 @@
       <c r="C7" s="575"/>
       <c r="D7" s="575"/>
       <c r="E7" s="608" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F7" s="568" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G7" s="567"/>
       <c r="H7" s="568"/>
@@ -34346,28 +34340,28 @@
         <v>233</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I8" s="600" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="J8" s="605" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="K8" s="606" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="L8" s="606" t="s">
         <v>529</v>
       </c>
       <c r="M8" s="607" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="N8" s="269" t="s">
         <v>368</v>
@@ -34379,16 +34373,16 @@
       <c r="D9" s="68"/>
       <c r="E9" s="609"/>
       <c r="F9" s="569" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="G9" s="569" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="H9" s="569" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="J9" s="21"/>
       <c r="K9" s="10"/>
@@ -34419,7 +34413,7 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="19" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F11" s="576"/>
       <c r="G11" s="576"/>
@@ -34446,7 +34440,7 @@
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="19" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F12" s="576"/>
       <c r="G12" s="576"/>
@@ -34473,7 +34467,7 @@
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="19" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F13" s="576"/>
       <c r="G13" s="576"/>
@@ -34500,7 +34494,7 @@
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F14" s="576"/>
       <c r="G14" s="576"/>
@@ -34530,7 +34524,7 @@
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="19" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F15" s="576"/>
       <c r="G15" s="576"/>
@@ -34557,7 +34551,7 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F16" s="576"/>
       <c r="G16" s="576"/>
@@ -34584,7 +34578,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="19" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F17" s="576"/>
       <c r="G17" s="576"/>
@@ -34611,7 +34605,7 @@
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="19" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F18" s="576"/>
       <c r="G18" s="576"/>
@@ -34638,7 +34632,7 @@
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="19" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F19" s="576"/>
       <c r="G19" s="576"/>
@@ -34665,7 +34659,7 @@
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="19" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F20" s="576"/>
       <c r="G20" s="576"/>
@@ -34692,7 +34686,7 @@
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="19" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F21" s="576"/>
       <c r="G21" s="576"/>
@@ -34719,7 +34713,7 @@
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="19" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F22" s="576"/>
       <c r="G22" s="576"/>
@@ -34793,7 +34787,7 @@
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="19" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F26" s="576"/>
       <c r="G26" s="576"/>
@@ -34820,7 +34814,7 @@
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="19" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F27" s="576"/>
       <c r="G27" s="576"/>
@@ -34847,7 +34841,7 @@
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="19" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F28" s="576"/>
       <c r="G28" s="576"/>
@@ -34874,7 +34868,7 @@
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="19" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="F29" s="576"/>
       <c r="G29" s="576"/>
@@ -34904,7 +34898,7 @@
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="19" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F30" s="576"/>
       <c r="G30" s="576"/>
@@ -34931,7 +34925,7 @@
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="19" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F31" s="576"/>
       <c r="G31" s="576"/>
@@ -34958,7 +34952,7 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="19" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F32" s="576"/>
       <c r="G32" s="576"/>
@@ -34985,7 +34979,7 @@
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="19" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="F33" s="576"/>
       <c r="G33" s="576"/>
@@ -35012,7 +35006,7 @@
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="19" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F34" s="576"/>
       <c r="G34" s="576"/>
@@ -35039,7 +35033,7 @@
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="19" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F35" s="576"/>
       <c r="G35" s="576"/>
@@ -35066,7 +35060,7 @@
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="19" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F36" s="576"/>
       <c r="G36" s="576"/>
@@ -35093,7 +35087,7 @@
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="19" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F37" s="576"/>
       <c r="G37" s="576"/>
@@ -35170,7 +35164,7 @@
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="19" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F41" s="576"/>
       <c r="G41" s="576"/>
@@ -35197,7 +35191,7 @@
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="19" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="F42" s="576"/>
       <c r="G42" s="576"/>
@@ -35224,7 +35218,7 @@
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F43" s="576"/>
       <c r="G43" s="576"/>
@@ -35283,7 +35277,7 @@
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="19" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F46" s="576"/>
       <c r="G46" s="576"/>
@@ -35310,7 +35304,7 @@
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F47" s="576"/>
       <c r="G47" s="576"/>
@@ -35337,7 +35331,7 @@
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="19" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F48" s="576"/>
       <c r="G48" s="576"/>
@@ -35364,7 +35358,7 @@
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="19" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F49" s="576"/>
       <c r="G49" s="576"/>
@@ -35391,7 +35385,7 @@
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="19" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F50" s="576"/>
       <c r="G50" s="576"/>
@@ -35450,7 +35444,7 @@
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="19" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F53" s="576"/>
       <c r="G53" s="576"/>
@@ -35474,7 +35468,7 @@
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="19" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F54" s="576"/>
       <c r="G54" s="576"/>
@@ -35498,7 +35492,7 @@
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F55" s="576"/>
       <c r="G55" s="576"/>

</xml_diff>

<commit_message>
Published state of ETDataset on 22 January 2016
</commit_message>
<xml_diff>
--- a/analyses/6_residences_analysis.xlsx
+++ b/analyses/6_residences_analysis.xlsx
@@ -57,45 +57,45 @@
   <definedNames>
     <definedName name="base_year">Dashboard!$E$12</definedName>
     <definedName name="country">Dashboard!$E$11</definedName>
-    <definedName name="Eff_cooking_biomass">technical_specs!$O$51</definedName>
-    <definedName name="Eff_cooking_electric">technical_specs!$O$48</definedName>
-    <definedName name="Eff_cooking_gas">technical_specs!$O$47</definedName>
-    <definedName name="Eff_cooking_halogen">technical_specs!$O$49</definedName>
-    <definedName name="Eff_cooking_induction">technical_specs!$O$50</definedName>
-    <definedName name="Eff_cooling_airco">technical_specs!$O$44</definedName>
-    <definedName name="Eff_cooling_pump_air">technical_specs!$O$43</definedName>
-    <definedName name="Eff_cooling_pump_ground">technical_specs!$O$42</definedName>
-    <definedName name="Eff_hot_water_coal">technical_specs!$O$36</definedName>
-    <definedName name="Eff_hot_water_combi_boiler">technical_specs!$O$26</definedName>
-    <definedName name="Eff_hot_water_district">technical_specs!$O$30</definedName>
-    <definedName name="Eff_hot_water_electric">technical_specs!$O$33</definedName>
-    <definedName name="Eff_hot_water_fuel_cell">technical_specs!$O$37</definedName>
-    <definedName name="Eff_hot_water_gas">technical_specs!$O$34</definedName>
-    <definedName name="Eff_hot_water_hhp_gas">technical_specs!$O$39</definedName>
-    <definedName name="Eff_hot_water_hhp_heatpump">technical_specs!$O$38</definedName>
-    <definedName name="Eff_hot_water_micro_CHP">technical_specs!$O$29</definedName>
-    <definedName name="Eff_hot_water_oil">technical_specs!$O$35</definedName>
-    <definedName name="Eff_hot_water_pump_air">technical_specs!$O$31</definedName>
-    <definedName name="Eff_hot_water_pump_ground">technical_specs!$O$28</definedName>
-    <definedName name="Eff_hot_water_solar_thermal_panel">technical_specs!$O$27</definedName>
-    <definedName name="Eff_hot_water_woodpellets">technical_specs!$O$32</definedName>
-    <definedName name="Eff_lighting_fluorescent">technical_specs!$O$55</definedName>
-    <definedName name="Eff_lighting_incandescent">technical_specs!$O$54</definedName>
-    <definedName name="Eff_lighting_led">technical_specs!$O$56</definedName>
-    <definedName name="Eff_space_heating_coal">technical_specs!$O$21</definedName>
-    <definedName name="Eff_space_heating_combi_boiler">technical_specs!$O$11</definedName>
-    <definedName name="Eff_space_heating_district">technical_specs!$O$15</definedName>
-    <definedName name="Eff_space_heating_electric">technical_specs!$O$18</definedName>
-    <definedName name="Eff_space_heating_gas">technical_specs!$O$19</definedName>
-    <definedName name="Eff_space_heating_hhp_gas">technical_specs!$O$23</definedName>
-    <definedName name="Eff_space_heating_hhp_heatpump">technical_specs!$O$22</definedName>
-    <definedName name="Eff_space_heating_micro_CHP">technical_specs!$O$14</definedName>
-    <definedName name="Eff_space_heating_oil">technical_specs!$O$20</definedName>
-    <definedName name="Eff_space_heating_pump_add_on">technical_specs!$O$22</definedName>
-    <definedName name="Eff_space_heating_pump_air">technical_specs!$O$16</definedName>
-    <definedName name="Eff_space_heating_pump_ground">technical_specs!$O$13</definedName>
-    <definedName name="Eff_space_heating_solar_thermal">technical_specs!$O$12</definedName>
-    <definedName name="Eff_space_heating_woodpellets">technical_specs!$O$17</definedName>
+    <definedName name="Eff_cooking_biomass">technical_specs!$P$51</definedName>
+    <definedName name="Eff_cooking_electric">technical_specs!$P$48</definedName>
+    <definedName name="Eff_cooking_gas">technical_specs!$P$47</definedName>
+    <definedName name="Eff_cooking_halogen">technical_specs!$P$49</definedName>
+    <definedName name="Eff_cooking_induction">technical_specs!$P$50</definedName>
+    <definedName name="Eff_cooling_airco">technical_specs!$P$44</definedName>
+    <definedName name="Eff_cooling_pump_air">technical_specs!$P$43</definedName>
+    <definedName name="Eff_cooling_pump_ground">technical_specs!$P$42</definedName>
+    <definedName name="Eff_hot_water_coal">technical_specs!$P$36</definedName>
+    <definedName name="Eff_hot_water_combi_boiler">technical_specs!$P$26</definedName>
+    <definedName name="Eff_hot_water_district">technical_specs!$P$30</definedName>
+    <definedName name="Eff_hot_water_electric">technical_specs!$P$33</definedName>
+    <definedName name="Eff_hot_water_fuel_cell">technical_specs!$P$37</definedName>
+    <definedName name="Eff_hot_water_gas">technical_specs!$P$34</definedName>
+    <definedName name="Eff_hot_water_hhp_gas">technical_specs!$P$39</definedName>
+    <definedName name="Eff_hot_water_hhp_heatpump">technical_specs!$P$38</definedName>
+    <definedName name="Eff_hot_water_micro_CHP">technical_specs!$P$29</definedName>
+    <definedName name="Eff_hot_water_oil">technical_specs!$P$35</definedName>
+    <definedName name="Eff_hot_water_pump_air">technical_specs!$P$31</definedName>
+    <definedName name="Eff_hot_water_pump_ground">technical_specs!$P$28</definedName>
+    <definedName name="Eff_hot_water_solar_thermal_panel">technical_specs!$P$27</definedName>
+    <definedName name="Eff_hot_water_woodpellets">technical_specs!$P$32</definedName>
+    <definedName name="Eff_lighting_fluorescent">technical_specs!$P$55</definedName>
+    <definedName name="Eff_lighting_incandescent">technical_specs!$P$54</definedName>
+    <definedName name="Eff_lighting_led">technical_specs!$P$56</definedName>
+    <definedName name="Eff_space_heating_coal">technical_specs!$P$21</definedName>
+    <definedName name="Eff_space_heating_combi_boiler">technical_specs!$P$11</definedName>
+    <definedName name="Eff_space_heating_district">technical_specs!$P$15</definedName>
+    <definedName name="Eff_space_heating_electric">technical_specs!$P$18</definedName>
+    <definedName name="Eff_space_heating_gas">technical_specs!$P$19</definedName>
+    <definedName name="Eff_space_heating_hhp_gas">technical_specs!$P$23</definedName>
+    <definedName name="Eff_space_heating_hhp_heatpump">technical_specs!$P$22</definedName>
+    <definedName name="Eff_space_heating_micro_CHP">technical_specs!$P$14</definedName>
+    <definedName name="Eff_space_heating_oil">technical_specs!$P$20</definedName>
+    <definedName name="Eff_space_heating_pump_add_on">technical_specs!$P$22</definedName>
+    <definedName name="Eff_space_heating_pump_air">technical_specs!$P$16</definedName>
+    <definedName name="Eff_space_heating_pump_ground">technical_specs!$P$13</definedName>
+    <definedName name="Eff_space_heating_solar_thermal">technical_specs!$P$12</definedName>
+    <definedName name="Eff_space_heating_woodpellets">technical_specs!$P$17</definedName>
     <definedName name="Final_demand_appliances">Dashboard!$E$25</definedName>
     <definedName name="Final_demand_coal">'Fuel aggregation'!$C$11</definedName>
     <definedName name="Final_demand_cooking">Dashboard!$E$24</definedName>
@@ -112,7 +112,7 @@
     <definedName name="Final_demand_space_heating">Dashboard!$E$20</definedName>
     <definedName name="Final_demand_woodpellets">'Fuel aggregation'!$F$11</definedName>
   </definedNames>
-  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="893">
   <si>
     <t>Changelog</t>
   </si>
@@ -2761,9 +2761,6 @@
     <t>network gas input</t>
   </si>
   <si>
-    <t>Input share network_gas</t>
-  </si>
-  <si>
     <t>Percentage of useful demand delivered per subtechnology (same as column D except for HHP)</t>
   </si>
   <si>
@@ -2819,6 +2816,15 @@
   </si>
   <si>
     <t>Percentage of useful heat in hot water delivered by solar thermal panel (if household is equipped)</t>
+  </si>
+  <si>
+    <t>heat efficiency gas subtechnology</t>
+  </si>
+  <si>
+    <t>output.useable_heat.network_gas</t>
+  </si>
+  <si>
+    <t>Heat output share network_gas</t>
   </si>
 </sst>
 </file>
@@ -15930,7 +15936,7 @@
     <row r="26" spans="2:13">
       <c r="B26" s="49"/>
       <c r="C26" s="276" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D26" s="640" t="e">
         <f>'Technology split final demand'!I22</f>
@@ -15952,7 +15958,7 @@
     <row r="27" spans="2:13">
       <c r="B27" s="49"/>
       <c r="C27" s="277" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D27" s="637" t="e">
         <f>'Technology split final demand'!I23</f>
@@ -15974,7 +15980,7 @@
     <row r="28" spans="2:13">
       <c r="B28" s="278"/>
       <c r="C28" s="639" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D28" s="155"/>
       <c r="E28" s="297"/>
@@ -17150,7 +17156,7 @@
         <v>462</v>
       </c>
       <c r="E9" s="82" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F9" s="82" t="s">
         <v>525</v>
@@ -17532,7 +17538,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="182">
-        <f>D22*(1-technical_specs!N23)</f>
+        <f>D22*(1-technical_specs!O23)</f>
         <v>0</v>
       </c>
       <c r="F22" s="561" t="e">
@@ -17560,7 +17566,7 @@
       </c>
       <c r="D23" s="182"/>
       <c r="E23" s="182">
-        <f>D22*technical_specs!N23</f>
+        <f>D22*technical_specs!O23</f>
         <v>0</v>
       </c>
       <c r="F23" s="561">
@@ -17989,7 +17995,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="182">
-        <f>D38*(1-technical_specs!N39)</f>
+        <f>D38*(1-technical_specs!O39)</f>
         <v>0</v>
       </c>
       <c r="F38" s="561" t="e">
@@ -18017,7 +18023,7 @@
       </c>
       <c r="D39" s="182"/>
       <c r="E39" s="182">
-        <f>D38*technical_specs!N39</f>
+        <f>D38*technical_specs!O39</f>
         <v>0</v>
       </c>
       <c r="F39" s="561">
@@ -18672,11 +18678,11 @@
         <v>Technology</v>
       </c>
       <c r="C9" s="68" t="str">
-        <f>technical_specs!K8</f>
+        <f>technical_specs!L8</f>
         <v>Heating efficiency</v>
       </c>
       <c r="D9" s="68" t="str">
-        <f>technical_specs!M8</f>
+        <f>technical_specs!N8</f>
         <v>Electrical efficiency</v>
       </c>
       <c r="E9" s="68" t="s">
@@ -18705,11 +18711,11 @@
         <v>Micro CHP (gas-fired)) (space heating)</v>
       </c>
       <c r="C11" s="210">
-        <f>technical_specs!K14</f>
+        <f>technical_specs!L14</f>
         <v>0</v>
       </c>
       <c r="D11" s="210">
-        <f>technical_specs!M14</f>
+        <f>technical_specs!N14</f>
         <v>0</v>
       </c>
       <c r="E11" s="210">
@@ -18732,11 +18738,11 @@
         <v>Micro CHP (gas-fired)) (hot water)</v>
       </c>
       <c r="C12" s="210">
-        <f>technical_specs!K29</f>
+        <f>technical_specs!L29</f>
         <v>0</v>
       </c>
       <c r="D12" s="210">
-        <f>technical_specs!M29</f>
+        <f>technical_specs!N29</f>
         <v>0</v>
       </c>
       <c r="E12" s="210">
@@ -18759,11 +18765,11 @@
         <v>Fuel Cell (hot water)</v>
       </c>
       <c r="C13" s="210">
-        <f>technical_specs!K37</f>
+        <f>technical_specs!L37</f>
         <v>0</v>
       </c>
       <c r="D13" s="210">
-        <f>technical_specs!M37</f>
+        <f>technical_specs!N37</f>
         <v>0</v>
       </c>
       <c r="E13" s="210">
@@ -19285,7 +19291,7 @@
         <v>215</v>
       </c>
       <c r="G9" s="217" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H9" s="217" t="s">
         <v>642</v>
@@ -19323,7 +19329,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F11" s="281">
-        <f>technical_specs!O11</f>
+        <f>technical_specs!P11</f>
         <v>0</v>
       </c>
       <c r="G11" s="644" t="e">
@@ -19357,7 +19363,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F12" s="281">
-        <f>technical_specs!O12</f>
+        <f>technical_specs!P12</f>
         <v>0</v>
       </c>
       <c r="G12" s="644" t="e">
@@ -19391,7 +19397,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F13" s="281" t="e">
-        <f>technical_specs!O13</f>
+        <f>technical_specs!P13</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G13" s="644" t="e">
@@ -19425,7 +19431,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F14" s="281">
-        <f>technical_specs!O14</f>
+        <f>technical_specs!P14</f>
         <v>0</v>
       </c>
       <c r="G14" s="644" t="e">
@@ -19459,7 +19465,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F15" s="281">
-        <f>technical_specs!O15</f>
+        <f>technical_specs!P15</f>
         <v>0</v>
       </c>
       <c r="G15" s="644" t="e">
@@ -19493,7 +19499,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F16" s="281" t="e">
-        <f>technical_specs!O16</f>
+        <f>technical_specs!P16</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G16" s="644" t="e">
@@ -19527,7 +19533,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F17" s="281">
-        <f>technical_specs!O17</f>
+        <f>technical_specs!P17</f>
         <v>0</v>
       </c>
       <c r="G17" s="644" t="e">
@@ -19561,7 +19567,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F18" s="281">
-        <f>technical_specs!O18</f>
+        <f>technical_specs!P18</f>
         <v>0</v>
       </c>
       <c r="G18" s="644" t="e">
@@ -19595,7 +19601,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F19" s="281">
-        <f>technical_specs!O19</f>
+        <f>technical_specs!P19</f>
         <v>0</v>
       </c>
       <c r="G19" s="644" t="e">
@@ -19629,7 +19635,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F20" s="281">
-        <f>technical_specs!O20</f>
+        <f>technical_specs!P20</f>
         <v>0</v>
       </c>
       <c r="G20" s="644" t="e">
@@ -19665,7 +19671,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F21" s="281">
-        <f>technical_specs!O21</f>
+        <f>technical_specs!P21</f>
         <v>0</v>
       </c>
       <c r="G21" s="644" t="e">
@@ -19701,7 +19707,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F22" s="281" t="e">
-        <f>technical_specs!O22</f>
+        <f>technical_specs!P22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G22" s="644" t="e">
@@ -19737,7 +19743,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F23" s="283">
-        <f>technical_specs!O23</f>
+        <f>technical_specs!P23</f>
         <v>0</v>
       </c>
       <c r="G23" s="645" t="e">
@@ -19805,7 +19811,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F26" s="281">
-        <f>technical_specs!O26</f>
+        <f>technical_specs!P26</f>
         <v>0</v>
       </c>
       <c r="G26" s="644" t="e">
@@ -19841,7 +19847,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F27" s="281">
-        <f>technical_specs!O27</f>
+        <f>technical_specs!P27</f>
         <v>0</v>
       </c>
       <c r="G27" s="644" t="e">
@@ -19877,7 +19883,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F28" s="281" t="e">
-        <f>technical_specs!O28</f>
+        <f>technical_specs!P28</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G28" s="644" t="e">
@@ -19913,7 +19919,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F29" s="281">
-        <f>technical_specs!O29</f>
+        <f>technical_specs!P29</f>
         <v>0</v>
       </c>
       <c r="G29" s="644" t="e">
@@ -19949,7 +19955,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F30" s="281">
-        <f>technical_specs!O30</f>
+        <f>technical_specs!P30</f>
         <v>0</v>
       </c>
       <c r="G30" s="644" t="e">
@@ -19985,7 +19991,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F31" s="281" t="e">
-        <f>technical_specs!O31</f>
+        <f>technical_specs!P31</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G31" s="644" t="e">
@@ -20021,7 +20027,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F32" s="281">
-        <f>technical_specs!O32</f>
+        <f>technical_specs!P32</f>
         <v>0</v>
       </c>
       <c r="G32" s="644" t="e">
@@ -20057,7 +20063,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F33" s="281">
-        <f>technical_specs!O33</f>
+        <f>technical_specs!P33</f>
         <v>0</v>
       </c>
       <c r="G33" s="644" t="e">
@@ -20093,7 +20099,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F34" s="281">
-        <f>technical_specs!O34</f>
+        <f>technical_specs!P34</f>
         <v>0</v>
       </c>
       <c r="G34" s="644" t="e">
@@ -20129,7 +20135,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F35" s="281">
-        <f>technical_specs!O35</f>
+        <f>technical_specs!P35</f>
         <v>0</v>
       </c>
       <c r="G35" s="644" t="e">
@@ -20165,7 +20171,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F36" s="281">
-        <f>technical_specs!O36</f>
+        <f>technical_specs!P36</f>
         <v>0</v>
       </c>
       <c r="G36" s="644" t="e">
@@ -20201,7 +20207,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F37" s="281">
-        <f>technical_specs!O37</f>
+        <f>technical_specs!P37</f>
         <v>0</v>
       </c>
       <c r="G37" s="644" t="e">
@@ -20237,7 +20243,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F38" s="281" t="e">
-        <f>technical_specs!O38</f>
+        <f>technical_specs!P38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G38" s="644" t="e">
@@ -20273,7 +20279,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F39" s="283">
-        <f>technical_specs!O39</f>
+        <f>technical_specs!P39</f>
         <v>0</v>
       </c>
       <c r="G39" s="645" t="e">
@@ -20356,7 +20362,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F43" s="281" t="e">
-        <f>technical_specs!O42</f>
+        <f>technical_specs!P42</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G43" s="644" t="e">
@@ -20392,7 +20398,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F44" s="281" t="e">
-        <f>technical_specs!O43</f>
+        <f>technical_specs!P43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G44" s="644" t="e">
@@ -20428,7 +20434,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F45" s="283" t="e">
-        <f>technical_specs!O44</f>
+        <f>technical_specs!P44</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G45" s="644" t="e">
@@ -20511,7 +20517,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F49" s="281">
-        <f>technical_specs!O47</f>
+        <f>technical_specs!P47</f>
         <v>0</v>
       </c>
       <c r="G49" s="644" t="e">
@@ -20547,7 +20553,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F50" s="281">
-        <f>technical_specs!O48</f>
+        <f>technical_specs!P48</f>
         <v>0</v>
       </c>
       <c r="G50" s="644" t="e">
@@ -20583,7 +20589,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F51" s="281">
-        <f>technical_specs!O49</f>
+        <f>technical_specs!P49</f>
         <v>0</v>
       </c>
       <c r="G51" s="644" t="e">
@@ -20619,7 +20625,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F52" s="281">
-        <f>technical_specs!O50</f>
+        <f>technical_specs!P50</f>
         <v>0</v>
       </c>
       <c r="G52" s="644" t="e">
@@ -20655,7 +20661,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F53" s="283">
-        <f>technical_specs!O51</f>
+        <f>technical_specs!P51</f>
         <v>0</v>
       </c>
       <c r="G53" s="644" t="e">
@@ -20738,7 +20744,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F57" s="281">
-        <f>technical_specs!O54</f>
+        <f>technical_specs!P54</f>
         <v>0</v>
       </c>
       <c r="G57" s="644" t="e">
@@ -20774,7 +20780,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F58" s="281">
-        <f>technical_specs!O55</f>
+        <f>technical_specs!P55</f>
         <v>0</v>
       </c>
       <c r="G58" s="644" t="e">
@@ -20810,7 +20816,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F59" s="283">
-        <f>technical_specs!O56</f>
+        <f>technical_specs!P56</f>
         <v>0</v>
       </c>
       <c r="G59" s="645" t="e">
@@ -21422,10 +21428,10 @@
     </row>
     <row r="35" spans="2:4" ht="30">
       <c r="B35" s="19" t="s">
+        <v>887</v>
+      </c>
+      <c r="C35" s="40" t="s">
         <v>888</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>889</v>
       </c>
       <c r="D35" s="18">
         <v>2.1800000000000002</v>
@@ -22051,7 +22057,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B7" s="190" t="e">
         <f>'Technology Shares'!F24</f>
@@ -22128,7 +22134,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B6" s="190" t="e">
         <f>'Technology Shares'!F29</f>
@@ -25655,7 +25661,7 @@
   </sheetPr>
   <dimension ref="B2:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
@@ -26591,7 +26597,7 @@
       <c r="M42" s="351"/>
       <c r="N42" s="75"/>
       <c r="O42" s="454" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="P42" s="451"/>
     </row>
@@ -26930,7 +26936,7 @@
       <c r="M58" s="351"/>
       <c r="N58" s="75"/>
       <c r="O58" s="454" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="P58" s="451"/>
     </row>
@@ -27691,7 +27697,7 @@
     <row r="95" spans="2:16" ht="16" thickBot="1">
       <c r="B95" s="38"/>
       <c r="C95" s="71" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D95" s="397"/>
       <c r="E95" s="390"/>
@@ -34980,10 +34986,10 @@
   <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:P58"/>
+  <dimension ref="B2:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -34994,19 +35000,20 @@
     <col min="4" max="4" width="16.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="64.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="17.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" style="119" customWidth="1"/>
-    <col min="16" max="16" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="29" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="17.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" style="119" customWidth="1"/>
+    <col min="17" max="17" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="20">
+    <row r="2" spans="2:17" ht="20">
       <c r="B2" s="63" t="s">
         <v>188</v>
       </c>
@@ -35018,8 +35025,9 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-    </row>
-    <row r="4" spans="2:16">
+      <c r="K2" s="8"/>
+    </row>
+    <row r="4" spans="2:17">
       <c r="B4" s="607" t="s">
         <v>79</v>
       </c>
@@ -35033,11 +35041,12 @@
       <c r="J4" s="612"/>
       <c r="K4" s="612"/>
       <c r="L4" s="612"/>
-      <c r="M4" s="8"/>
+      <c r="M4" s="612"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="187"/>
-    </row>
-    <row r="5" spans="2:16">
+      <c r="O4" s="8"/>
+      <c r="P4" s="187"/>
+    </row>
+    <row r="5" spans="2:17">
       <c r="B5" s="585" t="s">
         <v>797</v>
       </c>
@@ -35053,9 +35062,10 @@
       <c r="L5" s="149"/>
       <c r="M5" s="149"/>
       <c r="N5" s="149"/>
-      <c r="O5" s="187"/>
-    </row>
-    <row r="6" spans="2:16" ht="16" thickBot="1">
+      <c r="O5" s="149"/>
+      <c r="P5" s="187"/>
+    </row>
+    <row r="6" spans="2:17" ht="16" thickBot="1">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -35065,8 +35075,9 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="2:16">
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="2:17">
       <c r="B7" s="564" t="s">
         <v>643</v>
       </c>
@@ -35078,17 +35089,18 @@
       <c r="F7" s="558" t="s">
         <v>794</v>
       </c>
-      <c r="G7" s="557"/>
+      <c r="G7" s="558"/>
       <c r="H7" s="557"/>
-      <c r="I7" s="558"/>
-      <c r="J7" s="589"/>
-      <c r="K7" s="592"/>
-      <c r="L7" s="593"/>
+      <c r="I7" s="557"/>
+      <c r="J7" s="558"/>
+      <c r="K7" s="589"/>
+      <c r="L7" s="592"/>
       <c r="M7" s="593"/>
       <c r="N7" s="593"/>
-      <c r="O7" s="594"/>
-    </row>
-    <row r="8" spans="2:16" ht="30" customHeight="1">
+      <c r="O7" s="593"/>
+      <c r="P7" s="594"/>
+    </row>
+    <row r="8" spans="2:17" ht="30" customHeight="1">
       <c r="B8" s="587" t="s">
         <v>284</v>
       </c>
@@ -35103,37 +35115,40 @@
         <v>752</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>890</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>756</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>870</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>753</v>
       </c>
-      <c r="J8" s="590" t="s">
+      <c r="K8" s="590" t="s">
         <v>795</v>
       </c>
-      <c r="K8" s="595" t="s">
+      <c r="L8" s="595" t="s">
         <v>725</v>
       </c>
-      <c r="L8" s="596" t="s">
+      <c r="M8" s="596" t="s">
         <v>726</v>
       </c>
-      <c r="M8" s="596" t="s">
+      <c r="N8" s="596" t="s">
         <v>524</v>
       </c>
-      <c r="N8" s="596" t="s">
-        <v>871</v>
-      </c>
-      <c r="O8" s="597" t="s">
+      <c r="O8" s="596" t="s">
+        <v>892</v>
+      </c>
+      <c r="P8" s="597" t="s">
         <v>727</v>
       </c>
-      <c r="P8" s="268" t="s">
+      <c r="Q8" s="268" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="15" customHeight="1">
+    <row r="9" spans="2:17" ht="15" customHeight="1">
       <c r="B9" s="44"/>
       <c r="C9" s="10"/>
       <c r="D9" s="68"/>
@@ -35142,24 +35157,27 @@
         <v>754</v>
       </c>
       <c r="G9" s="559" t="s">
+        <v>891</v>
+      </c>
+      <c r="H9" s="559" t="s">
         <v>755</v>
       </c>
-      <c r="H9" s="559" t="s">
+      <c r="I9" s="559" t="s">
         <v>869</v>
       </c>
-      <c r="I9" s="559" t="s">
+      <c r="J9" s="559" t="s">
         <v>751</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>790</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="10"/>
+      <c r="L9" s="21"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="591"/>
-    </row>
-    <row r="10" spans="2:16">
+      <c r="O9" s="10"/>
+      <c r="P9" s="591"/>
+    </row>
+    <row r="10" spans="2:17">
       <c r="B10" s="49" t="s">
         <v>77</v>
       </c>
@@ -35170,15 +35188,16 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="70"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="138"/>
-      <c r="P10" s="268"/>
-    </row>
-    <row r="11" spans="2:16">
+      <c r="O10" s="8"/>
+      <c r="P10" s="138"/>
+      <c r="Q10" s="268"/>
+    </row>
+    <row r="11" spans="2:17">
       <c r="B11" s="49"/>
       <c r="C11" s="17" t="s">
         <v>409</v>
@@ -35191,23 +35210,24 @@
       <c r="G11" s="566"/>
       <c r="H11" s="566"/>
       <c r="I11" s="566"/>
-      <c r="J11" s="600"/>
-      <c r="K11" s="221">
+      <c r="J11" s="566"/>
+      <c r="K11" s="600"/>
+      <c r="L11" s="221">
         <f>F11</f>
         <v>0</v>
       </c>
-      <c r="L11" s="227"/>
-      <c r="M11" s="71"/>
+      <c r="M11" s="227"/>
       <c r="N11" s="71"/>
-      <c r="O11" s="228">
-        <f>K11</f>
+      <c r="O11" s="71"/>
+      <c r="P11" s="228">
+        <f>L11</f>
         <v>0</v>
       </c>
-      <c r="P11" s="268" t="s">
+      <c r="Q11" s="268" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:17">
       <c r="B12" s="49"/>
       <c r="C12" s="17" t="s">
         <v>415</v>
@@ -35220,23 +35240,24 @@
       <c r="G12" s="566"/>
       <c r="H12" s="566"/>
       <c r="I12" s="566"/>
-      <c r="J12" s="600"/>
-      <c r="K12" s="221">
+      <c r="J12" s="566"/>
+      <c r="K12" s="600"/>
+      <c r="L12" s="221">
         <f>F12</f>
         <v>0</v>
       </c>
-      <c r="L12" s="227"/>
-      <c r="M12" s="71"/>
+      <c r="M12" s="227"/>
       <c r="N12" s="71"/>
-      <c r="O12" s="228">
-        <f>K12</f>
+      <c r="O12" s="71"/>
+      <c r="P12" s="228">
+        <f>L12</f>
         <v>0</v>
       </c>
-      <c r="P12" s="268" t="s">
+      <c r="Q12" s="268" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:17">
       <c r="B13" s="49"/>
       <c r="C13" s="17" t="s">
         <v>411</v>
@@ -35249,23 +35270,24 @@
       <c r="G13" s="566"/>
       <c r="H13" s="566"/>
       <c r="I13" s="566"/>
-      <c r="J13" s="600"/>
-      <c r="K13" s="221"/>
-      <c r="L13" s="227" t="e">
-        <f>1/G13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="71"/>
+      <c r="J13" s="566"/>
+      <c r="K13" s="600"/>
+      <c r="L13" s="221"/>
+      <c r="M13" s="227" t="e">
+        <f>1/H13</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N13" s="71"/>
-      <c r="O13" s="228" t="e">
-        <f>L13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="268" t="s">
+      <c r="O13" s="71"/>
+      <c r="P13" s="228" t="e">
+        <f>M13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q13" s="268" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:17">
       <c r="B14" s="49"/>
       <c r="C14" s="17" t="s">
         <v>429</v>
@@ -35278,26 +35300,27 @@
       <c r="G14" s="566"/>
       <c r="H14" s="566"/>
       <c r="I14" s="566"/>
-      <c r="J14" s="600"/>
-      <c r="K14" s="221">
+      <c r="J14" s="566"/>
+      <c r="K14" s="600"/>
+      <c r="L14" s="221">
         <f>F14</f>
         <v>0</v>
       </c>
-      <c r="L14" s="227"/>
-      <c r="M14" s="493">
-        <f>I14</f>
+      <c r="M14" s="227"/>
+      <c r="N14" s="493">
+        <f>J14</f>
         <v>0</v>
       </c>
-      <c r="N14" s="493"/>
-      <c r="O14" s="228">
-        <f>K14</f>
+      <c r="O14" s="493"/>
+      <c r="P14" s="228">
+        <f>L14</f>
         <v>0</v>
       </c>
-      <c r="P14" s="268" t="s">
+      <c r="Q14" s="268" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:17">
       <c r="B15" s="49"/>
       <c r="C15" s="17" t="s">
         <v>414</v>
@@ -35310,23 +35333,24 @@
       <c r="G15" s="566"/>
       <c r="H15" s="566"/>
       <c r="I15" s="566"/>
-      <c r="J15" s="600"/>
-      <c r="K15" s="221">
+      <c r="J15" s="566"/>
+      <c r="K15" s="600"/>
+      <c r="L15" s="221">
         <f>F15</f>
         <v>0</v>
       </c>
-      <c r="L15" s="227"/>
-      <c r="M15" s="71"/>
+      <c r="M15" s="227"/>
       <c r="N15" s="71"/>
-      <c r="O15" s="228">
-        <f>K15</f>
+      <c r="O15" s="71"/>
+      <c r="P15" s="228">
+        <f>L15</f>
         <v>0</v>
       </c>
-      <c r="P15" s="268" t="s">
+      <c r="Q15" s="268" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:17">
       <c r="B16" s="67"/>
       <c r="C16" s="17" t="s">
         <v>416</v>
@@ -35339,23 +35363,24 @@
       <c r="G16" s="566"/>
       <c r="H16" s="566"/>
       <c r="I16" s="566"/>
-      <c r="J16" s="600"/>
-      <c r="K16" s="221"/>
-      <c r="L16" s="227" t="e">
-        <f>1/G16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="71"/>
+      <c r="J16" s="566"/>
+      <c r="K16" s="600"/>
+      <c r="L16" s="221"/>
+      <c r="M16" s="227" t="e">
+        <f>1/H16</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N16" s="71"/>
-      <c r="O16" s="228" t="e">
-        <f>L16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="268" t="s">
+      <c r="O16" s="71"/>
+      <c r="P16" s="228" t="e">
+        <f>M16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" s="268" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:17">
       <c r="B17" s="67"/>
       <c r="C17" s="17" t="s">
         <v>418</v>
@@ -35368,23 +35393,24 @@
       <c r="G17" s="566"/>
       <c r="H17" s="566"/>
       <c r="I17" s="566"/>
-      <c r="J17" s="600"/>
-      <c r="K17" s="221">
+      <c r="J17" s="566"/>
+      <c r="K17" s="600"/>
+      <c r="L17" s="221">
         <f>F17</f>
         <v>0</v>
       </c>
-      <c r="L17" s="227"/>
-      <c r="M17" s="71"/>
+      <c r="M17" s="227"/>
       <c r="N17" s="71"/>
-      <c r="O17" s="228">
-        <f>K17</f>
+      <c r="O17" s="71"/>
+      <c r="P17" s="228">
+        <f>L17</f>
         <v>0</v>
       </c>
-      <c r="P17" s="268" t="s">
+      <c r="Q17" s="268" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:17">
       <c r="B18" s="67"/>
       <c r="C18" s="17" t="s">
         <v>419</v>
@@ -35397,23 +35423,24 @@
       <c r="G18" s="566"/>
       <c r="H18" s="566"/>
       <c r="I18" s="566"/>
-      <c r="J18" s="600"/>
-      <c r="K18" s="221">
+      <c r="J18" s="566"/>
+      <c r="K18" s="600"/>
+      <c r="L18" s="221">
         <f>F18</f>
         <v>0</v>
       </c>
-      <c r="L18" s="227"/>
-      <c r="M18" s="71"/>
+      <c r="M18" s="227"/>
       <c r="N18" s="71"/>
-      <c r="O18" s="228">
-        <f>K18</f>
+      <c r="O18" s="71"/>
+      <c r="P18" s="228">
+        <f>L18</f>
         <v>0</v>
       </c>
-      <c r="P18" s="268" t="s">
+      <c r="Q18" s="268" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:17">
       <c r="B19" s="67"/>
       <c r="C19" s="17" t="s">
         <v>420</v>
@@ -35426,23 +35453,24 @@
       <c r="G19" s="566"/>
       <c r="H19" s="566"/>
       <c r="I19" s="566"/>
-      <c r="J19" s="600"/>
-      <c r="K19" s="221">
+      <c r="J19" s="566"/>
+      <c r="K19" s="600"/>
+      <c r="L19" s="221">
         <f>F19</f>
         <v>0</v>
       </c>
-      <c r="L19" s="227"/>
-      <c r="M19" s="71"/>
+      <c r="M19" s="227"/>
       <c r="N19" s="71"/>
-      <c r="O19" s="228">
-        <f>K19</f>
+      <c r="O19" s="71"/>
+      <c r="P19" s="228">
+        <f>L19</f>
         <v>0</v>
       </c>
-      <c r="P19" s="268" t="s">
+      <c r="Q19" s="268" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:17">
       <c r="B20" s="67"/>
       <c r="C20" s="17" t="s">
         <v>421</v>
@@ -35455,23 +35483,24 @@
       <c r="G20" s="566"/>
       <c r="H20" s="566"/>
       <c r="I20" s="566"/>
-      <c r="J20" s="600"/>
-      <c r="K20" s="221">
+      <c r="J20" s="566"/>
+      <c r="K20" s="600"/>
+      <c r="L20" s="221">
         <f>F20</f>
         <v>0</v>
       </c>
-      <c r="L20" s="227"/>
-      <c r="M20" s="71"/>
+      <c r="M20" s="227"/>
       <c r="N20" s="71"/>
-      <c r="O20" s="228">
-        <f>K20</f>
+      <c r="O20" s="71"/>
+      <c r="P20" s="228">
+        <f>L20</f>
         <v>0</v>
       </c>
-      <c r="P20" s="268" t="s">
+      <c r="Q20" s="268" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:17">
       <c r="B21" s="67"/>
       <c r="C21" s="17" t="s">
         <v>422</v>
@@ -35484,26 +35513,27 @@
       <c r="G21" s="566"/>
       <c r="H21" s="566"/>
       <c r="I21" s="566"/>
-      <c r="J21" s="600"/>
-      <c r="K21" s="221">
+      <c r="J21" s="566"/>
+      <c r="K21" s="600"/>
+      <c r="L21" s="221">
         <f>F21</f>
         <v>0</v>
       </c>
-      <c r="L21" s="227"/>
-      <c r="M21" s="71"/>
+      <c r="M21" s="227"/>
       <c r="N21" s="71"/>
-      <c r="O21" s="228">
-        <f>K21</f>
+      <c r="O21" s="71"/>
+      <c r="P21" s="228">
+        <f>L21</f>
         <v>0</v>
       </c>
-      <c r="P21" s="268" t="s">
+      <c r="Q21" s="268" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:17">
       <c r="B22" s="67"/>
       <c r="C22" s="17" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="19" t="s">
@@ -35513,68 +35543,73 @@
       <c r="G22" s="566"/>
       <c r="H22" s="566"/>
       <c r="I22" s="566"/>
-      <c r="J22" s="600"/>
-      <c r="K22" s="221"/>
-      <c r="L22" s="227" t="e">
-        <f>(1-H22)/G22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="71"/>
+      <c r="J22" s="566"/>
+      <c r="K22" s="600"/>
+      <c r="L22" s="221"/>
+      <c r="M22" s="227" t="e">
+        <f>(1-I22)/H22</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N22" s="71"/>
-      <c r="O22" s="228" t="e">
-        <f>L22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="268" t="s">
+      <c r="O22" s="71"/>
+      <c r="P22" s="228" t="e">
+        <f>M22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q22" s="268" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="23" spans="2:16">
+    <row r="23" spans="2:17">
       <c r="B23" s="67"/>
       <c r="C23" s="17" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="19"/>
       <c r="F23" s="566">
-        <f>F22</f>
+        <f t="shared" ref="F23:K23" si="0">F22</f>
         <v>0</v>
       </c>
       <c r="G23" s="566">
-        <f>G22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" s="566">
-        <f>H22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I23" s="566">
-        <f>I22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="600">
-        <f>J22</f>
+      <c r="J23" s="566">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="221">
-        <f>F23</f>
+      <c r="K23" s="600">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L23" s="227"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="566">
-        <f>H23</f>
+      <c r="L23" s="221">
+        <f>G23</f>
         <v>0</v>
       </c>
-      <c r="O23" s="228">
-        <f>K23</f>
+      <c r="M23" s="227"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="566">
+        <f>I23*G23</f>
         <v>0</v>
       </c>
-      <c r="P23" s="268" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16">
+      <c r="P23" s="228">
+        <f>L23</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="268" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
       <c r="B24" s="44"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -35583,15 +35618,16 @@
       <c r="G24" s="567"/>
       <c r="H24" s="567"/>
       <c r="I24" s="567"/>
-      <c r="J24" s="601"/>
-      <c r="K24" s="222"/>
-      <c r="L24" s="229"/>
-      <c r="M24" s="197"/>
+      <c r="J24" s="567"/>
+      <c r="K24" s="601"/>
+      <c r="L24" s="222"/>
+      <c r="M24" s="229"/>
       <c r="N24" s="197"/>
-      <c r="O24" s="230"/>
-      <c r="P24" s="220"/>
-    </row>
-    <row r="25" spans="2:16">
+      <c r="O24" s="197"/>
+      <c r="P24" s="230"/>
+      <c r="Q24" s="220"/>
+    </row>
+    <row r="25" spans="2:17">
       <c r="B25" s="49" t="s">
         <v>304</v>
       </c>
@@ -35602,15 +35638,16 @@
       <c r="G25" s="568"/>
       <c r="H25" s="568"/>
       <c r="I25" s="568"/>
-      <c r="J25" s="602"/>
-      <c r="K25" s="223"/>
-      <c r="L25" s="231"/>
-      <c r="M25" s="193"/>
+      <c r="J25" s="568"/>
+      <c r="K25" s="602"/>
+      <c r="L25" s="223"/>
+      <c r="M25" s="231"/>
       <c r="N25" s="193"/>
-      <c r="O25" s="232"/>
-      <c r="P25" s="220"/>
-    </row>
-    <row r="26" spans="2:16">
+      <c r="O25" s="193"/>
+      <c r="P25" s="232"/>
+      <c r="Q25" s="220"/>
+    </row>
+    <row r="26" spans="2:17">
       <c r="B26" s="49"/>
       <c r="C26" s="17" t="s">
         <v>410</v>
@@ -35623,23 +35660,24 @@
       <c r="G26" s="566"/>
       <c r="H26" s="566"/>
       <c r="I26" s="566"/>
-      <c r="J26" s="600"/>
-      <c r="K26" s="221">
+      <c r="J26" s="566"/>
+      <c r="K26" s="600"/>
+      <c r="L26" s="221">
         <f>F26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="227"/>
-      <c r="M26" s="71"/>
+      <c r="M26" s="227"/>
       <c r="N26" s="71"/>
-      <c r="O26" s="228">
-        <f>K26</f>
+      <c r="O26" s="71"/>
+      <c r="P26" s="228">
+        <f>L26</f>
         <v>0</v>
       </c>
-      <c r="P26" s="268" t="s">
+      <c r="Q26" s="268" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:17">
       <c r="B27" s="49"/>
       <c r="C27" s="17" t="s">
         <v>412</v>
@@ -35652,23 +35690,24 @@
       <c r="G27" s="566"/>
       <c r="H27" s="566"/>
       <c r="I27" s="566"/>
-      <c r="J27" s="600"/>
-      <c r="K27" s="221">
+      <c r="J27" s="566"/>
+      <c r="K27" s="600"/>
+      <c r="L27" s="221">
         <f>F27</f>
         <v>0</v>
       </c>
-      <c r="L27" s="209"/>
-      <c r="M27" s="142"/>
+      <c r="M27" s="209"/>
       <c r="N27" s="142"/>
-      <c r="O27" s="228">
-        <f>K27</f>
+      <c r="O27" s="142"/>
+      <c r="P27" s="228">
+        <f>L27</f>
         <v>0</v>
       </c>
-      <c r="P27" s="268" t="s">
+      <c r="Q27" s="268" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:17">
       <c r="B28" s="49"/>
       <c r="C28" s="17" t="s">
         <v>431</v>
@@ -35681,23 +35720,24 @@
       <c r="G28" s="566"/>
       <c r="H28" s="566"/>
       <c r="I28" s="566"/>
-      <c r="J28" s="600"/>
-      <c r="K28" s="221"/>
-      <c r="L28" s="227" t="e">
-        <f>1/G28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M28" s="71"/>
+      <c r="J28" s="566"/>
+      <c r="K28" s="600"/>
+      <c r="L28" s="221"/>
+      <c r="M28" s="227" t="e">
+        <f>1/H28</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N28" s="71"/>
-      <c r="O28" s="228" t="e">
-        <f>L28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="268" t="s">
+      <c r="O28" s="71"/>
+      <c r="P28" s="228" t="e">
+        <f>M28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q28" s="268" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:17">
       <c r="B29" s="49"/>
       <c r="C29" s="17" t="s">
         <v>430</v>
@@ -35710,26 +35750,27 @@
       <c r="G29" s="566"/>
       <c r="H29" s="566"/>
       <c r="I29" s="566"/>
-      <c r="J29" s="600"/>
-      <c r="K29" s="221">
+      <c r="J29" s="566"/>
+      <c r="K29" s="600"/>
+      <c r="L29" s="221">
         <f>F29</f>
         <v>0</v>
       </c>
-      <c r="L29" s="227"/>
-      <c r="M29" s="493">
-        <f>I29</f>
+      <c r="M29" s="227"/>
+      <c r="N29" s="493">
+        <f>J29</f>
         <v>0</v>
       </c>
-      <c r="N29" s="493"/>
-      <c r="O29" s="228">
-        <f>K29</f>
+      <c r="O29" s="493"/>
+      <c r="P29" s="228">
+        <f>L29</f>
         <v>0</v>
       </c>
-      <c r="P29" s="268" t="s">
+      <c r="Q29" s="268" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:17">
       <c r="B30" s="49"/>
       <c r="C30" s="17" t="s">
         <v>413</v>
@@ -35742,23 +35783,24 @@
       <c r="G30" s="566"/>
       <c r="H30" s="566"/>
       <c r="I30" s="566"/>
-      <c r="J30" s="600"/>
-      <c r="K30" s="221">
+      <c r="J30" s="566"/>
+      <c r="K30" s="600"/>
+      <c r="L30" s="221">
         <f>F30</f>
         <v>0</v>
       </c>
-      <c r="L30" s="227"/>
-      <c r="M30" s="71"/>
+      <c r="M30" s="227"/>
       <c r="N30" s="71"/>
-      <c r="O30" s="228">
-        <f>K30</f>
+      <c r="O30" s="71"/>
+      <c r="P30" s="228">
+        <f>L30</f>
         <v>0</v>
       </c>
-      <c r="P30" s="268" t="s">
+      <c r="Q30" s="268" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:17">
       <c r="B31" s="67"/>
       <c r="C31" s="17" t="s">
         <v>417</v>
@@ -35771,23 +35813,24 @@
       <c r="G31" s="566"/>
       <c r="H31" s="566"/>
       <c r="I31" s="566"/>
-      <c r="J31" s="600"/>
-      <c r="K31" s="221"/>
-      <c r="L31" s="227" t="e">
-        <f>1/G31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" s="71"/>
+      <c r="J31" s="566"/>
+      <c r="K31" s="600"/>
+      <c r="L31" s="221"/>
+      <c r="M31" s="227" t="e">
+        <f>1/H31</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N31" s="71"/>
-      <c r="O31" s="228" t="e">
-        <f>L31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="268" t="s">
+      <c r="O31" s="71"/>
+      <c r="P31" s="228" t="e">
+        <f>M31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q31" s="268" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="2:16">
+    <row r="32" spans="2:17">
       <c r="B32" s="67"/>
       <c r="C32" s="17" t="s">
         <v>423</v>
@@ -35800,23 +35843,24 @@
       <c r="G32" s="566"/>
       <c r="H32" s="566"/>
       <c r="I32" s="566"/>
-      <c r="J32" s="600"/>
-      <c r="K32" s="221">
-        <f t="shared" ref="K32:K37" si="0">F32</f>
+      <c r="J32" s="566"/>
+      <c r="K32" s="600"/>
+      <c r="L32" s="221">
+        <f t="shared" ref="L32:L37" si="1">F32</f>
         <v>0</v>
       </c>
-      <c r="L32" s="227"/>
-      <c r="M32" s="71"/>
+      <c r="M32" s="227"/>
       <c r="N32" s="71"/>
-      <c r="O32" s="228">
-        <f t="shared" ref="O32:O36" si="1">K32</f>
+      <c r="O32" s="71"/>
+      <c r="P32" s="228">
+        <f t="shared" ref="P32:P36" si="2">L32</f>
         <v>0</v>
       </c>
-      <c r="P32" s="268" t="s">
+      <c r="Q32" s="268" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="2:16">
+    <row r="33" spans="2:17">
       <c r="B33" s="67"/>
       <c r="C33" s="17" t="s">
         <v>424</v>
@@ -35829,23 +35873,24 @@
       <c r="G33" s="566"/>
       <c r="H33" s="566"/>
       <c r="I33" s="566"/>
-      <c r="J33" s="600"/>
-      <c r="K33" s="221">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="227"/>
-      <c r="M33" s="71"/>
-      <c r="N33" s="71"/>
-      <c r="O33" s="228">
+      <c r="J33" s="566"/>
+      <c r="K33" s="600"/>
+      <c r="L33" s="221">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P33" s="268" t="s">
+      <c r="M33" s="227"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="228">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="268" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="2:16">
+    <row r="34" spans="2:17">
       <c r="B34" s="67"/>
       <c r="C34" s="17" t="s">
         <v>425</v>
@@ -35858,23 +35903,24 @@
       <c r="G34" s="566"/>
       <c r="H34" s="566"/>
       <c r="I34" s="566"/>
-      <c r="J34" s="600"/>
-      <c r="K34" s="221">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="227"/>
-      <c r="M34" s="71"/>
-      <c r="N34" s="71"/>
-      <c r="O34" s="228">
+      <c r="J34" s="566"/>
+      <c r="K34" s="600"/>
+      <c r="L34" s="221">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P34" s="268" t="s">
+      <c r="M34" s="227"/>
+      <c r="N34" s="71"/>
+      <c r="O34" s="71"/>
+      <c r="P34" s="228">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="268" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="35" spans="2:16">
+    <row r="35" spans="2:17">
       <c r="B35" s="67"/>
       <c r="C35" s="17" t="s">
         <v>426</v>
@@ -35887,23 +35933,24 @@
       <c r="G35" s="566"/>
       <c r="H35" s="566"/>
       <c r="I35" s="566"/>
-      <c r="J35" s="600"/>
-      <c r="K35" s="221">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="227"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="71"/>
-      <c r="O35" s="228">
+      <c r="J35" s="566"/>
+      <c r="K35" s="600"/>
+      <c r="L35" s="221">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P35" s="268" t="s">
+      <c r="M35" s="227"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="228">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="268" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="36" spans="2:16">
+    <row r="36" spans="2:17">
       <c r="B36" s="67"/>
       <c r="C36" s="17" t="s">
         <v>427</v>
@@ -35916,23 +35963,24 @@
       <c r="G36" s="566"/>
       <c r="H36" s="566"/>
       <c r="I36" s="566"/>
-      <c r="J36" s="600"/>
-      <c r="K36" s="221">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="227"/>
-      <c r="M36" s="71"/>
-      <c r="N36" s="71"/>
-      <c r="O36" s="228">
+      <c r="J36" s="566"/>
+      <c r="K36" s="600"/>
+      <c r="L36" s="221">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P36" s="268" t="s">
+      <c r="M36" s="227"/>
+      <c r="N36" s="71"/>
+      <c r="O36" s="71"/>
+      <c r="P36" s="228">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="268" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="37" spans="2:16">
+    <row r="37" spans="2:17">
       <c r="B37" s="67"/>
       <c r="C37" s="17" t="s">
         <v>428</v>
@@ -35945,100 +35993,106 @@
       <c r="G37" s="566"/>
       <c r="H37" s="566"/>
       <c r="I37" s="566"/>
-      <c r="J37" s="600"/>
-      <c r="K37" s="221">
-        <f t="shared" si="0"/>
+      <c r="J37" s="566"/>
+      <c r="K37" s="600"/>
+      <c r="L37" s="221">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L37" s="227"/>
-      <c r="M37" s="493">
-        <f>I37</f>
+      <c r="M37" s="227"/>
+      <c r="N37" s="493">
+        <f>J37</f>
         <v>0</v>
       </c>
-      <c r="N37" s="493"/>
-      <c r="O37" s="228">
-        <f>K37</f>
+      <c r="O37" s="493"/>
+      <c r="P37" s="228">
+        <f>L37</f>
         <v>0</v>
       </c>
-      <c r="P37" s="268" t="s">
+      <c r="Q37" s="268" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="38" spans="2:16">
+    <row r="38" spans="2:17">
       <c r="B38" s="67"/>
       <c r="C38" s="17" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="19" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F38" s="566"/>
       <c r="G38" s="566"/>
       <c r="H38" s="566"/>
       <c r="I38" s="566"/>
-      <c r="J38" s="600"/>
-      <c r="K38" s="221"/>
-      <c r="L38" s="227" t="e">
-        <f>(1-H38)/G38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M38" s="493"/>
+      <c r="J38" s="566"/>
+      <c r="K38" s="600"/>
+      <c r="L38" s="221"/>
+      <c r="M38" s="227" t="e">
+        <f>(1-I38)/H38</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N38" s="493"/>
-      <c r="O38" s="228" t="e">
-        <f>L38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P38" s="268" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16">
+      <c r="O38" s="493"/>
+      <c r="P38" s="228" t="e">
+        <f>M38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q38" s="268" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17">
       <c r="B39" s="67"/>
       <c r="C39" s="17" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D39" s="17"/>
       <c r="E39" s="19"/>
       <c r="F39" s="566">
-        <f>F38</f>
+        <f t="shared" ref="F39:K39" si="3">F38</f>
         <v>0</v>
       </c>
       <c r="G39" s="566">
-        <f>G38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H39" s="566">
-        <f>H38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I39" s="566">
-        <f>I38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J39" s="600">
-        <f>J38</f>
+      <c r="J39" s="566">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K39" s="221">
-        <f>F39</f>
+      <c r="K39" s="600">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L39" s="227"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="566">
-        <f>H39</f>
+      <c r="L39" s="221">
+        <f>G39</f>
         <v>0</v>
       </c>
-      <c r="O39" s="228">
-        <f>K39</f>
+      <c r="M39" s="227"/>
+      <c r="N39" s="71"/>
+      <c r="O39" s="566">
+        <f>I39*G39</f>
         <v>0</v>
       </c>
-      <c r="P39" s="268" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16">
+      <c r="P39" s="228">
+        <f>L39</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="268" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17">
       <c r="B40" s="31"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -36047,15 +36101,16 @@
       <c r="G40" s="568"/>
       <c r="H40" s="568"/>
       <c r="I40" s="568"/>
-      <c r="J40" s="602"/>
-      <c r="K40" s="224"/>
-      <c r="L40" s="231"/>
-      <c r="M40" s="193"/>
+      <c r="J40" s="568"/>
+      <c r="K40" s="602"/>
+      <c r="L40" s="224"/>
+      <c r="M40" s="231"/>
       <c r="N40" s="193"/>
-      <c r="O40" s="233"/>
-      <c r="P40" s="220"/>
-    </row>
-    <row r="41" spans="2:16">
+      <c r="O40" s="193"/>
+      <c r="P40" s="233"/>
+      <c r="Q40" s="220"/>
+    </row>
+    <row r="41" spans="2:17">
       <c r="B41" s="48" t="s">
         <v>89</v>
       </c>
@@ -36066,15 +36121,16 @@
       <c r="G41" s="569"/>
       <c r="H41" s="569"/>
       <c r="I41" s="569"/>
-      <c r="J41" s="603"/>
-      <c r="K41" s="225"/>
-      <c r="L41" s="234"/>
-      <c r="M41" s="202"/>
+      <c r="J41" s="569"/>
+      <c r="K41" s="603"/>
+      <c r="L41" s="225"/>
+      <c r="M41" s="234"/>
       <c r="N41" s="202"/>
-      <c r="O41" s="235"/>
-      <c r="P41" s="220"/>
-    </row>
-    <row r="42" spans="2:16">
+      <c r="O41" s="202"/>
+      <c r="P41" s="235"/>
+      <c r="Q41" s="220"/>
+    </row>
+    <row r="42" spans="2:17">
       <c r="B42" s="67"/>
       <c r="C42" s="17" t="s">
         <v>345</v>
@@ -36087,23 +36143,24 @@
       <c r="G42" s="566"/>
       <c r="H42" s="566"/>
       <c r="I42" s="566"/>
-      <c r="J42" s="600"/>
-      <c r="K42" s="221"/>
-      <c r="L42" s="227" t="e">
-        <f>1/G42</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M42" s="71"/>
+      <c r="J42" s="566"/>
+      <c r="K42" s="600"/>
+      <c r="L42" s="221"/>
+      <c r="M42" s="227" t="e">
+        <f>1/H42</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N42" s="71"/>
-      <c r="O42" s="228" t="e">
-        <f>L42</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P42" s="268" t="s">
+      <c r="O42" s="71"/>
+      <c r="P42" s="228" t="e">
+        <f>M42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q42" s="268" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="43" spans="2:16">
+    <row r="43" spans="2:17">
       <c r="B43" s="67"/>
       <c r="C43" s="17" t="s">
         <v>344</v>
@@ -36116,23 +36173,24 @@
       <c r="G43" s="566"/>
       <c r="H43" s="566"/>
       <c r="I43" s="566"/>
-      <c r="J43" s="600"/>
-      <c r="K43" s="221"/>
-      <c r="L43" s="227" t="e">
-        <f>1/G43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M43" s="71"/>
+      <c r="J43" s="566"/>
+      <c r="K43" s="600"/>
+      <c r="L43" s="221"/>
+      <c r="M43" s="227" t="e">
+        <f>1/H43</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N43" s="71"/>
-      <c r="O43" s="228" t="e">
-        <f>L43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P43" s="268" t="s">
+      <c r="O43" s="71"/>
+      <c r="P43" s="228" t="e">
+        <f>M43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q43" s="268" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="44" spans="2:16">
+    <row r="44" spans="2:17">
       <c r="B44" s="67"/>
       <c r="C44" s="17" t="s">
         <v>346</v>
@@ -36145,23 +36203,24 @@
       <c r="G44" s="566"/>
       <c r="H44" s="566"/>
       <c r="I44" s="566"/>
-      <c r="J44" s="600"/>
-      <c r="K44" s="221"/>
-      <c r="L44" s="227" t="e">
-        <f>1/G44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M44" s="71"/>
+      <c r="J44" s="566"/>
+      <c r="K44" s="600"/>
+      <c r="L44" s="221"/>
+      <c r="M44" s="227" t="e">
+        <f>1/H44</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N44" s="71"/>
-      <c r="O44" s="228" t="e">
-        <f>L44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P44" s="268" t="s">
+      <c r="O44" s="71"/>
+      <c r="P44" s="228" t="e">
+        <f>M44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q44" s="268" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:17">
       <c r="B45" s="44"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -36170,15 +36229,16 @@
       <c r="G45" s="567"/>
       <c r="H45" s="567"/>
       <c r="I45" s="567"/>
-      <c r="J45" s="601"/>
-      <c r="K45" s="222"/>
-      <c r="L45" s="229"/>
-      <c r="M45" s="197"/>
+      <c r="J45" s="567"/>
+      <c r="K45" s="601"/>
+      <c r="L45" s="222"/>
+      <c r="M45" s="229"/>
       <c r="N45" s="197"/>
-      <c r="O45" s="230"/>
-      <c r="P45" s="220"/>
-    </row>
-    <row r="46" spans="2:16">
+      <c r="O45" s="197"/>
+      <c r="P45" s="230"/>
+      <c r="Q45" s="220"/>
+    </row>
+    <row r="46" spans="2:17">
       <c r="B46" s="49" t="s">
         <v>281</v>
       </c>
@@ -36189,15 +36249,16 @@
       <c r="G46" s="568"/>
       <c r="H46" s="568"/>
       <c r="I46" s="568"/>
-      <c r="J46" s="602"/>
-      <c r="K46" s="223"/>
-      <c r="L46" s="231"/>
-      <c r="M46" s="193"/>
+      <c r="J46" s="568"/>
+      <c r="K46" s="602"/>
+      <c r="L46" s="223"/>
+      <c r="M46" s="231"/>
       <c r="N46" s="193"/>
-      <c r="O46" s="232"/>
-      <c r="P46" s="220"/>
-    </row>
-    <row r="47" spans="2:16">
+      <c r="O46" s="193"/>
+      <c r="P46" s="232"/>
+      <c r="Q46" s="220"/>
+    </row>
+    <row r="47" spans="2:17">
       <c r="B47" s="49"/>
       <c r="C47" s="17" t="s">
         <v>355</v>
@@ -36210,23 +36271,24 @@
       <c r="G47" s="566"/>
       <c r="H47" s="566"/>
       <c r="I47" s="566"/>
-      <c r="J47" s="600"/>
-      <c r="K47" s="221">
+      <c r="J47" s="566"/>
+      <c r="K47" s="600"/>
+      <c r="L47" s="221">
         <f>F47</f>
         <v>0</v>
       </c>
-      <c r="L47" s="227"/>
-      <c r="M47" s="71"/>
+      <c r="M47" s="227"/>
       <c r="N47" s="71"/>
-      <c r="O47" s="228">
-        <f>K47</f>
+      <c r="O47" s="71"/>
+      <c r="P47" s="228">
+        <f>L47</f>
         <v>0</v>
       </c>
-      <c r="P47" s="268" t="s">
+      <c r="Q47" s="268" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="48" spans="2:16">
+    <row r="48" spans="2:17">
       <c r="B48" s="49"/>
       <c r="C48" s="17" t="s">
         <v>405</v>
@@ -36239,23 +36301,24 @@
       <c r="G48" s="566"/>
       <c r="H48" s="566"/>
       <c r="I48" s="566"/>
-      <c r="J48" s="600"/>
-      <c r="K48" s="221">
+      <c r="J48" s="566"/>
+      <c r="K48" s="600"/>
+      <c r="L48" s="221">
         <f>F48</f>
         <v>0</v>
       </c>
-      <c r="L48" s="227"/>
-      <c r="M48" s="71"/>
+      <c r="M48" s="227"/>
       <c r="N48" s="71"/>
-      <c r="O48" s="228">
-        <f t="shared" ref="O48:O51" si="2">K48</f>
+      <c r="O48" s="71"/>
+      <c r="P48" s="228">
+        <f t="shared" ref="P48:P51" si="4">L48</f>
         <v>0</v>
       </c>
-      <c r="P48" s="268" t="s">
+      <c r="Q48" s="268" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:17">
       <c r="B49" s="49"/>
       <c r="C49" s="17" t="s">
         <v>356</v>
@@ -36268,23 +36331,24 @@
       <c r="G49" s="566"/>
       <c r="H49" s="566"/>
       <c r="I49" s="566"/>
-      <c r="J49" s="600"/>
-      <c r="K49" s="221">
+      <c r="J49" s="566"/>
+      <c r="K49" s="600"/>
+      <c r="L49" s="221">
         <f>F49</f>
         <v>0</v>
       </c>
-      <c r="L49" s="227"/>
-      <c r="M49" s="71"/>
+      <c r="M49" s="227"/>
       <c r="N49" s="71"/>
-      <c r="O49" s="228">
-        <f t="shared" si="2"/>
+      <c r="O49" s="71"/>
+      <c r="P49" s="228">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P49" s="268" t="s">
+      <c r="Q49" s="268" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:17">
       <c r="B50" s="49"/>
       <c r="C50" s="17" t="s">
         <v>357</v>
@@ -36297,23 +36361,24 @@
       <c r="G50" s="566"/>
       <c r="H50" s="566"/>
       <c r="I50" s="566"/>
-      <c r="J50" s="600"/>
-      <c r="K50" s="221">
+      <c r="J50" s="566"/>
+      <c r="K50" s="600"/>
+      <c r="L50" s="221">
         <f>F50</f>
         <v>0</v>
       </c>
-      <c r="L50" s="227"/>
-      <c r="M50" s="71"/>
+      <c r="M50" s="227"/>
       <c r="N50" s="71"/>
-      <c r="O50" s="228">
-        <f t="shared" si="2"/>
+      <c r="O50" s="71"/>
+      <c r="P50" s="228">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P50" s="268" t="s">
+      <c r="Q50" s="268" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:17">
       <c r="B51" s="67"/>
       <c r="C51" s="17" t="s">
         <v>358</v>
@@ -36326,23 +36391,24 @@
       <c r="G51" s="566"/>
       <c r="H51" s="566"/>
       <c r="I51" s="566"/>
-      <c r="J51" s="600"/>
-      <c r="K51" s="221">
+      <c r="J51" s="566"/>
+      <c r="K51" s="600"/>
+      <c r="L51" s="221">
         <f>F51</f>
         <v>0</v>
       </c>
-      <c r="L51" s="227"/>
-      <c r="M51" s="71"/>
+      <c r="M51" s="227"/>
       <c r="N51" s="71"/>
-      <c r="O51" s="228">
-        <f t="shared" si="2"/>
+      <c r="O51" s="71"/>
+      <c r="P51" s="228">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P51" s="268" t="s">
+      <c r="Q51" s="268" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:17">
       <c r="B52" s="118"/>
       <c r="C52" s="45"/>
       <c r="D52" s="45"/>
@@ -36351,15 +36417,16 @@
       <c r="G52" s="570"/>
       <c r="H52" s="570"/>
       <c r="I52" s="570"/>
-      <c r="J52" s="605"/>
-      <c r="K52" s="226"/>
-      <c r="L52" s="236"/>
-      <c r="M52" s="237"/>
+      <c r="J52" s="570"/>
+      <c r="K52" s="605"/>
+      <c r="L52" s="226"/>
+      <c r="M52" s="236"/>
       <c r="N52" s="237"/>
-      <c r="O52" s="238"/>
-      <c r="P52" s="220"/>
-    </row>
-    <row r="53" spans="2:16">
+      <c r="O52" s="237"/>
+      <c r="P52" s="238"/>
+      <c r="Q52" s="220"/>
+    </row>
+    <row r="53" spans="2:17">
       <c r="B53" s="38" t="s">
         <v>76</v>
       </c>
@@ -36370,15 +36437,16 @@
       <c r="G53" s="568"/>
       <c r="H53" s="568"/>
       <c r="I53" s="568"/>
-      <c r="J53" s="602"/>
-      <c r="K53" s="224"/>
-      <c r="L53" s="231"/>
-      <c r="M53" s="193"/>
+      <c r="J53" s="568"/>
+      <c r="K53" s="602"/>
+      <c r="L53" s="224"/>
+      <c r="M53" s="231"/>
       <c r="N53" s="193"/>
-      <c r="O53" s="233"/>
-      <c r="P53" s="220"/>
-    </row>
-    <row r="54" spans="2:16">
+      <c r="O53" s="193"/>
+      <c r="P53" s="233"/>
+      <c r="Q53" s="220"/>
+    </row>
+    <row r="54" spans="2:17">
       <c r="B54" s="67"/>
       <c r="C54" s="17" t="s">
         <v>99</v>
@@ -36391,20 +36459,21 @@
       <c r="G54" s="566"/>
       <c r="H54" s="566"/>
       <c r="I54" s="566"/>
-      <c r="J54" s="600"/>
-      <c r="K54" s="221"/>
-      <c r="L54" s="227"/>
-      <c r="M54" s="71"/>
+      <c r="J54" s="566"/>
+      <c r="K54" s="600"/>
+      <c r="L54" s="221"/>
+      <c r="M54" s="227"/>
       <c r="N54" s="71"/>
-      <c r="O54" s="560">
-        <f>J54</f>
+      <c r="O54" s="71"/>
+      <c r="P54" s="560">
+        <f>K54</f>
         <v>0</v>
       </c>
-      <c r="P54" s="268" t="s">
+      <c r="Q54" s="268" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:17">
       <c r="B55" s="67"/>
       <c r="C55" s="17" t="s">
         <v>351</v>
@@ -36417,20 +36486,21 @@
       <c r="G55" s="566"/>
       <c r="H55" s="566"/>
       <c r="I55" s="566"/>
-      <c r="J55" s="600"/>
-      <c r="K55" s="221"/>
-      <c r="L55" s="227"/>
-      <c r="M55" s="71"/>
+      <c r="J55" s="566"/>
+      <c r="K55" s="600"/>
+      <c r="L55" s="221"/>
+      <c r="M55" s="227"/>
       <c r="N55" s="71"/>
-      <c r="O55" s="560">
-        <f>J55</f>
+      <c r="O55" s="71"/>
+      <c r="P55" s="560">
+        <f>K55</f>
         <v>0</v>
       </c>
-      <c r="P55" s="268" t="s">
+      <c r="Q55" s="268" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:17">
       <c r="B56" s="67"/>
       <c r="C56" s="17" t="s">
         <v>100</v>
@@ -36443,20 +36513,21 @@
       <c r="G56" s="566"/>
       <c r="H56" s="566"/>
       <c r="I56" s="566"/>
-      <c r="J56" s="600"/>
-      <c r="K56" s="221"/>
-      <c r="L56" s="227"/>
-      <c r="M56" s="71"/>
+      <c r="J56" s="566"/>
+      <c r="K56" s="600"/>
+      <c r="L56" s="221"/>
+      <c r="M56" s="227"/>
       <c r="N56" s="71"/>
-      <c r="O56" s="560">
-        <f>J56</f>
+      <c r="O56" s="71"/>
+      <c r="P56" s="560">
+        <f>K56</f>
         <v>0</v>
       </c>
-      <c r="P56" s="268" t="s">
+      <c r="Q56" s="268" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="2:16" ht="16" thickBot="1">
+    <row r="57" spans="2:17" ht="16" thickBot="1">
       <c r="B57" s="47"/>
       <c r="C57" s="77"/>
       <c r="D57" s="77"/>
@@ -36465,25 +36536,27 @@
       <c r="G57" s="571"/>
       <c r="H57" s="571"/>
       <c r="I57" s="571"/>
-      <c r="J57" s="606"/>
-      <c r="K57" s="129"/>
-      <c r="L57" s="77"/>
+      <c r="J57" s="571"/>
+      <c r="K57" s="606"/>
+      <c r="L57" s="129"/>
       <c r="M57" s="77"/>
       <c r="N57" s="77"/>
-      <c r="O57" s="139"/>
-    </row>
-    <row r="58" spans="2:16">
+      <c r="O57" s="77"/>
+      <c r="P57" s="139"/>
+    </row>
+    <row r="58" spans="2:17">
       <c r="F58" s="572"/>
       <c r="G58" s="572"/>
       <c r="H58" s="572"/>
       <c r="I58" s="572"/>
       <c r="J58" s="572"/>
+      <c r="K58" s="572"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="O31 O13:O16" formula="1"/>
+    <ignoredError sqref="P31 P13:P16" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>